<commit_message>
Update python visual demo.,
Signed-off-by: Jiamin Ma <jiamin.ma_2@nxp.com>
</commit_message>
<xml_diff>
--- a/python_visiaul/owner.xlsx
+++ b/python_visiaul/owner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.174.135\nxf32270\Misc_demo\python_visiaul\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9596AF88-7AED-4EFB-8A14-16183F9E2889}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2842D7D-3153-4B5A-9C09-47B45B73A401}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="SYS_BOOT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="423">
   <si>
     <t>NAME</t>
   </si>
@@ -1286,6 +1286,9 @@
   </si>
   <si>
     <t>UT-Exception</t>
+  </si>
+  <si>
+    <t>UT-Exception_A35</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2240,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD350"/>
+  <dimension ref="A1:AD351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10452,6 +10455,32 @@
         <v>38</v>
       </c>
     </row>
+    <row r="351" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A351" t="s">
+        <v>422</v>
+      </c>
+      <c r="B351" t="s">
+        <v>33</v>
+      </c>
+      <c r="C351" t="s">
+        <v>407</v>
+      </c>
+      <c r="E351" t="s">
+        <v>35</v>
+      </c>
+      <c r="M351">
+        <v>1</v>
+      </c>
+      <c r="W351" t="s">
+        <v>50</v>
+      </c>
+      <c r="X351" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y351" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>